<commit_message>
added note and excel sheet
</commit_message>
<xml_diff>
--- a/static/files/data.xlsx
+++ b/static/files/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,20 +446,25 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>chem_id</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>email</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>mob_number</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>is_workshop</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>is_iit_madras</t>
         </is>
@@ -481,18 +486,59 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>CHES210005</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>vivek17212797@gmail.com</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>8340447063</t>
         </is>
       </c>
-      <c r="F2" t="b">
+      <c r="G2" t="b">
         <v>0</v>
       </c>
-      <c r="G2" t="b">
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Ajinkya</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Kamble</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CHES210006</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>amartyakumar982@gmail.com</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>12345667</t>
+        </is>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>